<commit_message>
creates csv's, begins make_metadata draft
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_fish_observations_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_fish_observations_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9461D787-FF83-435D-BEAC-94344BFC3169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9FB6D6-6F29-4788-91C2-15342CD96080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,8 +196,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,10 +285,10 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -519,7 +519,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
fixes errors, validates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/feather_snorkel_fish_observations_metadata.xlsx
+++ b/data-raw/metadata/feather_snorkel_fish_observations_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\edi-feather-snorkel\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9FB6D6-6F29-4788-91C2-15342CD96080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70025E8-A0D8-41C2-93FC-7AA62774C59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -515,11 +515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z967"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1085,32 +1085,89 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+    </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
@@ -1118,27 +1175,27 @@
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -1169,6 +1226,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
       <c r="K19" s="2"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1327,6 +1394,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
@@ -1382,6 +1450,7 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="2"/>
@@ -1801,7 +1870,7 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
+      <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
@@ -1829,7 +1898,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
+      <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
@@ -1857,7 +1926,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
+      <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
@@ -1885,7 +1954,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+      <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
@@ -1913,7 +1982,7 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+      <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
@@ -1941,7 +2010,7 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
+      <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
@@ -1969,7 +2038,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
+      <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
@@ -1997,7 +2066,7 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4"/>
+      <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
@@ -2025,7 +2094,7 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="4"/>
+      <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="2"/>
@@ -2053,7 +2122,7 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="4"/>
+      <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="2"/>
@@ -2081,7 +2150,7 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
+      <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="2"/>
@@ -2109,7 +2178,7 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
+      <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
@@ -2137,7 +2206,7 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
+      <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="2"/>
@@ -2165,7 +2234,7 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
+      <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="2"/>
@@ -2193,7 +2262,7 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4"/>
+      <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
@@ -2221,7 +2290,7 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
+      <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="2"/>
@@ -2249,7 +2318,7 @@
       <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
+      <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="2"/>
@@ -2277,7 +2346,7 @@
       <c r="Z58" s="1"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
+      <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="2"/>
@@ -2305,7 +2374,7 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="2"/>
@@ -2333,7 +2402,7 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
+      <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="2"/>
@@ -27728,578 +27797,18 @@
       <c r="Y967" s="1"/>
       <c r="Z967" s="1"/>
     </row>
-    <row r="968" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A968" s="1"/>
-      <c r="B968" s="1"/>
-      <c r="C968" s="1"/>
-      <c r="D968" s="2"/>
-      <c r="E968" s="1"/>
-      <c r="F968" s="3"/>
-      <c r="G968" s="3"/>
-      <c r="H968" s="3"/>
-      <c r="I968" s="2"/>
-      <c r="J968" s="3"/>
-      <c r="K968" s="2"/>
-      <c r="L968" s="3"/>
-      <c r="M968" s="3"/>
-      <c r="N968" s="1"/>
-      <c r="O968" s="1"/>
-      <c r="P968" s="1"/>
-      <c r="Q968" s="1"/>
-      <c r="R968" s="1"/>
-      <c r="S968" s="1"/>
-      <c r="T968" s="1"/>
-      <c r="U968" s="1"/>
-      <c r="V968" s="1"/>
-      <c r="W968" s="1"/>
-      <c r="X968" s="1"/>
-      <c r="Y968" s="1"/>
-      <c r="Z968" s="1"/>
-    </row>
-    <row r="969" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A969" s="1"/>
-      <c r="B969" s="1"/>
-      <c r="C969" s="1"/>
-      <c r="D969" s="2"/>
-      <c r="E969" s="1"/>
-      <c r="F969" s="3"/>
-      <c r="G969" s="3"/>
-      <c r="H969" s="3"/>
-      <c r="I969" s="2"/>
-      <c r="J969" s="3"/>
-      <c r="K969" s="2"/>
-      <c r="L969" s="3"/>
-      <c r="M969" s="3"/>
-      <c r="N969" s="1"/>
-      <c r="O969" s="1"/>
-      <c r="P969" s="1"/>
-      <c r="Q969" s="1"/>
-      <c r="R969" s="1"/>
-      <c r="S969" s="1"/>
-      <c r="T969" s="1"/>
-      <c r="U969" s="1"/>
-      <c r="V969" s="1"/>
-      <c r="W969" s="1"/>
-      <c r="X969" s="1"/>
-      <c r="Y969" s="1"/>
-      <c r="Z969" s="1"/>
-    </row>
-    <row r="970" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A970" s="1"/>
-      <c r="B970" s="1"/>
-      <c r="C970" s="1"/>
-      <c r="D970" s="2"/>
-      <c r="E970" s="1"/>
-      <c r="F970" s="3"/>
-      <c r="G970" s="3"/>
-      <c r="H970" s="3"/>
-      <c r="I970" s="2"/>
-      <c r="J970" s="3"/>
-      <c r="K970" s="2"/>
-      <c r="L970" s="3"/>
-      <c r="M970" s="3"/>
-      <c r="N970" s="1"/>
-      <c r="O970" s="1"/>
-      <c r="P970" s="1"/>
-      <c r="Q970" s="1"/>
-      <c r="R970" s="1"/>
-      <c r="S970" s="1"/>
-      <c r="T970" s="1"/>
-      <c r="U970" s="1"/>
-      <c r="V970" s="1"/>
-      <c r="W970" s="1"/>
-      <c r="X970" s="1"/>
-      <c r="Y970" s="1"/>
-      <c r="Z970" s="1"/>
-    </row>
-    <row r="971" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A971" s="1"/>
-      <c r="B971" s="1"/>
-      <c r="C971" s="1"/>
-      <c r="D971" s="2"/>
-      <c r="E971" s="1"/>
-      <c r="F971" s="3"/>
-      <c r="G971" s="3"/>
-      <c r="H971" s="3"/>
-      <c r="I971" s="2"/>
-      <c r="J971" s="3"/>
-      <c r="K971" s="2"/>
-      <c r="L971" s="3"/>
-      <c r="M971" s="3"/>
-      <c r="N971" s="1"/>
-      <c r="O971" s="1"/>
-      <c r="P971" s="1"/>
-      <c r="Q971" s="1"/>
-      <c r="R971" s="1"/>
-      <c r="S971" s="1"/>
-      <c r="T971" s="1"/>
-      <c r="U971" s="1"/>
-      <c r="V971" s="1"/>
-      <c r="W971" s="1"/>
-      <c r="X971" s="1"/>
-      <c r="Y971" s="1"/>
-      <c r="Z971" s="1"/>
-    </row>
-    <row r="972" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A972" s="1"/>
-      <c r="B972" s="1"/>
-      <c r="C972" s="1"/>
-      <c r="D972" s="2"/>
-      <c r="E972" s="1"/>
-      <c r="F972" s="3"/>
-      <c r="G972" s="3"/>
-      <c r="H972" s="3"/>
-      <c r="I972" s="2"/>
-      <c r="J972" s="3"/>
-      <c r="K972" s="2"/>
-      <c r="L972" s="3"/>
-      <c r="M972" s="3"/>
-      <c r="N972" s="1"/>
-      <c r="O972" s="1"/>
-      <c r="P972" s="1"/>
-      <c r="Q972" s="1"/>
-      <c r="R972" s="1"/>
-      <c r="S972" s="1"/>
-      <c r="T972" s="1"/>
-      <c r="U972" s="1"/>
-      <c r="V972" s="1"/>
-      <c r="W972" s="1"/>
-      <c r="X972" s="1"/>
-      <c r="Y972" s="1"/>
-      <c r="Z972" s="1"/>
-    </row>
-    <row r="973" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A973" s="1"/>
-      <c r="B973" s="1"/>
-      <c r="C973" s="1"/>
-      <c r="D973" s="2"/>
-      <c r="E973" s="1"/>
-      <c r="F973" s="3"/>
-      <c r="G973" s="3"/>
-      <c r="H973" s="3"/>
-      <c r="I973" s="2"/>
-      <c r="J973" s="3"/>
-      <c r="K973" s="2"/>
-      <c r="L973" s="3"/>
-      <c r="M973" s="3"/>
-      <c r="N973" s="1"/>
-      <c r="O973" s="1"/>
-      <c r="P973" s="1"/>
-      <c r="Q973" s="1"/>
-      <c r="R973" s="1"/>
-      <c r="S973" s="1"/>
-      <c r="T973" s="1"/>
-      <c r="U973" s="1"/>
-      <c r="V973" s="1"/>
-      <c r="W973" s="1"/>
-      <c r="X973" s="1"/>
-      <c r="Y973" s="1"/>
-      <c r="Z973" s="1"/>
-    </row>
-    <row r="974" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A974" s="1"/>
-      <c r="B974" s="1"/>
-      <c r="C974" s="1"/>
-      <c r="D974" s="2"/>
-      <c r="E974" s="1"/>
-      <c r="F974" s="3"/>
-      <c r="G974" s="3"/>
-      <c r="H974" s="3"/>
-      <c r="I974" s="2"/>
-      <c r="J974" s="3"/>
-      <c r="K974" s="2"/>
-      <c r="L974" s="3"/>
-      <c r="M974" s="3"/>
-      <c r="N974" s="1"/>
-      <c r="O974" s="1"/>
-      <c r="P974" s="1"/>
-      <c r="Q974" s="1"/>
-      <c r="R974" s="1"/>
-      <c r="S974" s="1"/>
-      <c r="T974" s="1"/>
-      <c r="U974" s="1"/>
-      <c r="V974" s="1"/>
-      <c r="W974" s="1"/>
-      <c r="X974" s="1"/>
-      <c r="Y974" s="1"/>
-      <c r="Z974" s="1"/>
-    </row>
-    <row r="975" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A975" s="1"/>
-      <c r="B975" s="1"/>
-      <c r="C975" s="1"/>
-      <c r="D975" s="2"/>
-      <c r="E975" s="1"/>
-      <c r="F975" s="3"/>
-      <c r="G975" s="3"/>
-      <c r="H975" s="3"/>
-      <c r="I975" s="2"/>
-      <c r="J975" s="3"/>
-      <c r="K975" s="2"/>
-      <c r="L975" s="3"/>
-      <c r="M975" s="3"/>
-      <c r="N975" s="1"/>
-      <c r="O975" s="1"/>
-      <c r="P975" s="1"/>
-      <c r="Q975" s="1"/>
-      <c r="R975" s="1"/>
-      <c r="S975" s="1"/>
-      <c r="T975" s="1"/>
-      <c r="U975" s="1"/>
-      <c r="V975" s="1"/>
-      <c r="W975" s="1"/>
-      <c r="X975" s="1"/>
-      <c r="Y975" s="1"/>
-      <c r="Z975" s="1"/>
-    </row>
-    <row r="976" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A976" s="1"/>
-      <c r="B976" s="1"/>
-      <c r="C976" s="1"/>
-      <c r="D976" s="2"/>
-      <c r="E976" s="1"/>
-      <c r="F976" s="3"/>
-      <c r="G976" s="3"/>
-      <c r="H976" s="3"/>
-      <c r="I976" s="2"/>
-      <c r="J976" s="3"/>
-      <c r="K976" s="2"/>
-      <c r="L976" s="3"/>
-      <c r="M976" s="3"/>
-      <c r="N976" s="1"/>
-      <c r="O976" s="1"/>
-      <c r="P976" s="1"/>
-      <c r="Q976" s="1"/>
-      <c r="R976" s="1"/>
-      <c r="S976" s="1"/>
-      <c r="T976" s="1"/>
-      <c r="U976" s="1"/>
-      <c r="V976" s="1"/>
-      <c r="W976" s="1"/>
-      <c r="X976" s="1"/>
-      <c r="Y976" s="1"/>
-      <c r="Z976" s="1"/>
-    </row>
-    <row r="977" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A977" s="1"/>
-      <c r="B977" s="1"/>
-      <c r="C977" s="1"/>
-      <c r="D977" s="2"/>
-      <c r="E977" s="1"/>
-      <c r="F977" s="3"/>
-      <c r="G977" s="3"/>
-      <c r="H977" s="3"/>
-      <c r="I977" s="2"/>
-      <c r="J977" s="3"/>
-      <c r="K977" s="2"/>
-      <c r="L977" s="3"/>
-      <c r="M977" s="3"/>
-      <c r="N977" s="1"/>
-      <c r="O977" s="1"/>
-      <c r="P977" s="1"/>
-      <c r="Q977" s="1"/>
-      <c r="R977" s="1"/>
-      <c r="S977" s="1"/>
-      <c r="T977" s="1"/>
-      <c r="U977" s="1"/>
-      <c r="V977" s="1"/>
-      <c r="W977" s="1"/>
-      <c r="X977" s="1"/>
-      <c r="Y977" s="1"/>
-      <c r="Z977" s="1"/>
-    </row>
-    <row r="978" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A978" s="1"/>
-      <c r="B978" s="1"/>
-      <c r="C978" s="1"/>
-      <c r="D978" s="2"/>
-      <c r="E978" s="1"/>
-      <c r="F978" s="3"/>
-      <c r="G978" s="3"/>
-      <c r="H978" s="3"/>
-      <c r="I978" s="2"/>
-      <c r="J978" s="3"/>
-      <c r="K978" s="2"/>
-      <c r="L978" s="3"/>
-      <c r="M978" s="3"/>
-      <c r="N978" s="1"/>
-      <c r="O978" s="1"/>
-      <c r="P978" s="1"/>
-      <c r="Q978" s="1"/>
-      <c r="R978" s="1"/>
-      <c r="S978" s="1"/>
-      <c r="T978" s="1"/>
-      <c r="U978" s="1"/>
-      <c r="V978" s="1"/>
-      <c r="W978" s="1"/>
-      <c r="X978" s="1"/>
-      <c r="Y978" s="1"/>
-      <c r="Z978" s="1"/>
-    </row>
-    <row r="979" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A979" s="1"/>
-      <c r="B979" s="1"/>
-      <c r="C979" s="1"/>
-      <c r="D979" s="2"/>
-      <c r="E979" s="1"/>
-      <c r="F979" s="3"/>
-      <c r="G979" s="3"/>
-      <c r="H979" s="3"/>
-      <c r="I979" s="2"/>
-      <c r="J979" s="3"/>
-      <c r="K979" s="2"/>
-      <c r="L979" s="3"/>
-      <c r="M979" s="3"/>
-      <c r="N979" s="1"/>
-      <c r="O979" s="1"/>
-      <c r="P979" s="1"/>
-      <c r="Q979" s="1"/>
-      <c r="R979" s="1"/>
-      <c r="S979" s="1"/>
-      <c r="T979" s="1"/>
-      <c r="U979" s="1"/>
-      <c r="V979" s="1"/>
-      <c r="W979" s="1"/>
-      <c r="X979" s="1"/>
-      <c r="Y979" s="1"/>
-      <c r="Z979" s="1"/>
-    </row>
-    <row r="980" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A980" s="1"/>
-      <c r="B980" s="1"/>
-      <c r="C980" s="1"/>
-      <c r="D980" s="2"/>
-      <c r="E980" s="1"/>
-      <c r="F980" s="3"/>
-      <c r="G980" s="3"/>
-      <c r="H980" s="3"/>
-      <c r="I980" s="2"/>
-      <c r="J980" s="3"/>
-      <c r="K980" s="2"/>
-      <c r="L980" s="3"/>
-      <c r="M980" s="3"/>
-      <c r="N980" s="1"/>
-      <c r="O980" s="1"/>
-      <c r="P980" s="1"/>
-      <c r="Q980" s="1"/>
-      <c r="R980" s="1"/>
-      <c r="S980" s="1"/>
-      <c r="T980" s="1"/>
-      <c r="U980" s="1"/>
-      <c r="V980" s="1"/>
-      <c r="W980" s="1"/>
-      <c r="X980" s="1"/>
-      <c r="Y980" s="1"/>
-      <c r="Z980" s="1"/>
-    </row>
-    <row r="981" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A981" s="1"/>
-      <c r="B981" s="1"/>
-      <c r="C981" s="1"/>
-      <c r="D981" s="2"/>
-      <c r="E981" s="1"/>
-      <c r="F981" s="3"/>
-      <c r="G981" s="3"/>
-      <c r="H981" s="3"/>
-      <c r="I981" s="2"/>
-      <c r="J981" s="3"/>
-      <c r="K981" s="2"/>
-      <c r="L981" s="3"/>
-      <c r="M981" s="3"/>
-      <c r="N981" s="1"/>
-      <c r="O981" s="1"/>
-      <c r="P981" s="1"/>
-      <c r="Q981" s="1"/>
-      <c r="R981" s="1"/>
-      <c r="S981" s="1"/>
-      <c r="T981" s="1"/>
-      <c r="U981" s="1"/>
-      <c r="V981" s="1"/>
-      <c r="W981" s="1"/>
-      <c r="X981" s="1"/>
-      <c r="Y981" s="1"/>
-      <c r="Z981" s="1"/>
-    </row>
-    <row r="982" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A982" s="1"/>
-      <c r="B982" s="1"/>
-      <c r="C982" s="1"/>
-      <c r="D982" s="2"/>
-      <c r="E982" s="1"/>
-      <c r="F982" s="3"/>
-      <c r="G982" s="3"/>
-      <c r="H982" s="3"/>
-      <c r="I982" s="2"/>
-      <c r="J982" s="3"/>
-      <c r="K982" s="2"/>
-      <c r="L982" s="3"/>
-      <c r="M982" s="3"/>
-      <c r="N982" s="1"/>
-      <c r="O982" s="1"/>
-      <c r="P982" s="1"/>
-      <c r="Q982" s="1"/>
-      <c r="R982" s="1"/>
-      <c r="S982" s="1"/>
-      <c r="T982" s="1"/>
-      <c r="U982" s="1"/>
-      <c r="V982" s="1"/>
-      <c r="W982" s="1"/>
-      <c r="X982" s="1"/>
-      <c r="Y982" s="1"/>
-      <c r="Z982" s="1"/>
-    </row>
-    <row r="983" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A983" s="1"/>
-      <c r="B983" s="1"/>
-      <c r="C983" s="1"/>
-      <c r="D983" s="2"/>
-      <c r="E983" s="1"/>
-      <c r="F983" s="3"/>
-      <c r="G983" s="3"/>
-      <c r="H983" s="3"/>
-      <c r="I983" s="2"/>
-      <c r="J983" s="3"/>
-      <c r="K983" s="2"/>
-      <c r="L983" s="3"/>
-      <c r="M983" s="3"/>
-      <c r="N983" s="1"/>
-      <c r="O983" s="1"/>
-      <c r="P983" s="1"/>
-      <c r="Q983" s="1"/>
-      <c r="R983" s="1"/>
-      <c r="S983" s="1"/>
-      <c r="T983" s="1"/>
-      <c r="U983" s="1"/>
-      <c r="V983" s="1"/>
-      <c r="W983" s="1"/>
-      <c r="X983" s="1"/>
-      <c r="Y983" s="1"/>
-      <c r="Z983" s="1"/>
-    </row>
-    <row r="984" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A984" s="1"/>
-      <c r="B984" s="1"/>
-      <c r="C984" s="1"/>
-      <c r="D984" s="2"/>
-      <c r="E984" s="1"/>
-      <c r="F984" s="3"/>
-      <c r="G984" s="3"/>
-      <c r="H984" s="3"/>
-      <c r="I984" s="2"/>
-      <c r="J984" s="3"/>
-      <c r="K984" s="2"/>
-      <c r="L984" s="3"/>
-      <c r="M984" s="3"/>
-      <c r="N984" s="1"/>
-      <c r="O984" s="1"/>
-      <c r="P984" s="1"/>
-      <c r="Q984" s="1"/>
-      <c r="R984" s="1"/>
-      <c r="S984" s="1"/>
-      <c r="T984" s="1"/>
-      <c r="U984" s="1"/>
-      <c r="V984" s="1"/>
-      <c r="W984" s="1"/>
-      <c r="X984" s="1"/>
-      <c r="Y984" s="1"/>
-      <c r="Z984" s="1"/>
-    </row>
-    <row r="985" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A985" s="1"/>
-      <c r="B985" s="1"/>
-      <c r="C985" s="1"/>
-      <c r="D985" s="2"/>
-      <c r="E985" s="1"/>
-      <c r="F985" s="3"/>
-      <c r="G985" s="3"/>
-      <c r="H985" s="3"/>
-      <c r="I985" s="2"/>
-      <c r="J985" s="3"/>
-      <c r="K985" s="2"/>
-      <c r="L985" s="3"/>
-      <c r="M985" s="3"/>
-      <c r="N985" s="1"/>
-      <c r="O985" s="1"/>
-      <c r="P985" s="1"/>
-      <c r="Q985" s="1"/>
-      <c r="R985" s="1"/>
-      <c r="S985" s="1"/>
-      <c r="T985" s="1"/>
-      <c r="U985" s="1"/>
-      <c r="V985" s="1"/>
-      <c r="W985" s="1"/>
-      <c r="X985" s="1"/>
-      <c r="Y985" s="1"/>
-      <c r="Z985" s="1"/>
-    </row>
-    <row r="986" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A986" s="1"/>
-      <c r="B986" s="1"/>
-      <c r="C986" s="1"/>
-      <c r="D986" s="2"/>
-      <c r="E986" s="1"/>
-      <c r="F986" s="3"/>
-      <c r="G986" s="3"/>
-      <c r="H986" s="3"/>
-      <c r="I986" s="2"/>
-      <c r="J986" s="3"/>
-      <c r="K986" s="2"/>
-      <c r="L986" s="3"/>
-      <c r="M986" s="3"/>
-      <c r="N986" s="1"/>
-      <c r="O986" s="1"/>
-      <c r="P986" s="1"/>
-      <c r="Q986" s="1"/>
-      <c r="R986" s="1"/>
-      <c r="S986" s="1"/>
-      <c r="T986" s="1"/>
-      <c r="U986" s="1"/>
-      <c r="V986" s="1"/>
-      <c r="W986" s="1"/>
-      <c r="X986" s="1"/>
-      <c r="Y986" s="1"/>
-      <c r="Z986" s="1"/>
-    </row>
-    <row r="987" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A987" s="1"/>
-      <c r="B987" s="1"/>
-      <c r="C987" s="1"/>
-      <c r="D987" s="2"/>
-      <c r="E987" s="1"/>
-      <c r="F987" s="3"/>
-      <c r="G987" s="3"/>
-      <c r="H987" s="3"/>
-      <c r="I987" s="2"/>
-      <c r="J987" s="3"/>
-      <c r="K987" s="2"/>
-      <c r="L987" s="3"/>
-      <c r="M987" s="3"/>
-      <c r="N987" s="1"/>
-      <c r="O987" s="1"/>
-      <c r="P987" s="1"/>
-      <c r="Q987" s="1"/>
-      <c r="R987" s="1"/>
-      <c r="S987" s="1"/>
-      <c r="T987" s="1"/>
-      <c r="U987" s="1"/>
-      <c r="V987" s="1"/>
-      <c r="W987" s="1"/>
-      <c r="X987" s="1"/>
-      <c r="Y987" s="1"/>
-      <c r="Z987" s="1"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C44:C987 C20:C32 C16:C18 C1:C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C24:C967 C1:C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E20:E987 E16:E18 E1:E13" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E1:E967" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F20:F987 F16:F18 F1:F13" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F1:F967" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H987 H16:H18 H1:H13" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H1:H967" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>